<commit_message>
add rezult test distance
</commit_message>
<xml_diff>
--- a/test/wired_wireless_test.xlsx
+++ b/test/wired_wireless_test.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>distance, m</t>
   </si>
   <si>
-    <t>Δt</t>
+    <t>measuring, min</t>
+  </si>
+  <si>
+    <t>Δt, ms</t>
+  </si>
+  <si>
+    <t>Conclusion: Δt does not depend on the distance between the modules</t>
   </si>
 </sst>
 </file>
@@ -368,48 +374,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>